<commit_message>
Fix merge detection, ignore empty rows, test more edge cases
</commit_message>
<xml_diff>
--- a/examples/xlsx/foo.xlsx
+++ b/examples/xlsx/foo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ladeo/dev/arrai/examples/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47150E32-7014-EF45-BA17-891E9F9C4BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECC8EF-E90F-104B-936B-801AED8E15C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="3760" windowWidth="26840" windowHeight="15940" xr2:uid="{DA4A7C36-6721-9E4F-8108-DA4880905709}"/>
   </bookViews>
@@ -25,27 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Customer ID</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>foo</t>
   </si>
   <si>
     <t>bar</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>Checking</t>
   </si>
   <si>
     <t>Savings</t>
+  </si>
+  <si>
+    <t>ignored</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>Empty rows ignored</t>
+  </si>
+  <si>
+    <t>No header skipped</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>Commas ignored</t>
+  </si>
+  <si>
+    <t>Account, Balance</t>
+  </si>
+  <si>
+    <t>AccountType</t>
   </si>
 </sst>
 </file>
@@ -83,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,11 +121,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -114,6 +144,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,63 +462,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960BAB09-B5F1-9E44-9EE4-DD588BAF0124}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>300</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add docs alongside test foo.xlsx
</commit_message>
<xml_diff>
--- a/examples/xlsx/foo.xlsx
+++ b/examples/xlsx/foo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ladeo/dev/arrai/examples/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECC8EF-E90F-104B-936B-801AED8E15C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F325DA-167C-2E4D-973E-95F4CF64FD77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="3760" windowWidth="26840" windowHeight="15940" xr2:uid="{DA4A7C36-6721-9E4F-8108-DA4880905709}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Customer ID</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>empty</t>
-  </si>
-  <si>
-    <t>header</t>
   </si>
   <si>
     <t>Empty rows ignored</t>
@@ -465,7 +462,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,11 +477,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -501,15 +498,12 @@
         <v>100</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -520,13 +514,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -552,5 +546,6 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add extra arg to customise header row in case it's not zero
</commit_message>
<xml_diff>
--- a/examples/xlsx/foo.xlsx
+++ b/examples/xlsx/foo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ladeo/dev/arrai/examples/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F325DA-167C-2E4D-973E-95F4CF64FD77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D64E2D-0A82-7B4C-A54C-E17B3D130960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="3760" windowWidth="26840" windowHeight="15940" xr2:uid="{DA4A7C36-6721-9E4F-8108-DA4880905709}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Customer ID</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>AccountType</t>
+  </si>
+  <si>
+    <t>Non-heading</t>
+  </si>
+  <si>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -139,11 +145,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960BAB09-B5F1-9E44-9EE4-DD588BAF0124}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,77 +479,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>